<commit_message>
Prophet hyperparmater tuning done
</commit_message>
<xml_diff>
--- a/Prophet/Performance Metric - MAE.xlsx
+++ b/Prophet/Performance Metric - MAE.xlsx
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.6661127402474974</v>
+        <v>0.4147712986052281</v>
       </c>
     </row>
     <row r="3">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1014305725509313</v>
+        <v>0.09999565895742606</v>
       </c>
     </row>
     <row r="4">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.500278915241627</v>
+        <v>0.2021875542765255</v>
       </c>
     </row>
     <row r="5">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.1077541551709751</v>
+        <v>0.1029787273645813</v>
       </c>
     </row>
     <row r="7">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.2655428799490947</v>
+        <v>0.2350353010065291</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.2690356419371498</v>
+        <v>0.1326798583002398</v>
       </c>
     </row>
     <row r="9">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3368032718712705</v>
+        <v>0.3293286587327779</v>
       </c>
     </row>
     <row r="10">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.53000918868094</v>
+        <v>0.1755939442914869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>